<commit_message>
[Challenge 4] Redone charts
</commit_message>
<xml_diff>
--- a/challenge4/challenge4.xlsx
+++ b/challenge4/challenge4.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/p3700621/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/p3700621/Coding/big-data-yelp-challenge/challenge4/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,15 +30,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>AZ</t>
-  </si>
-  <si>
-    <t>BW</t>
-  </si>
-  <si>
-    <t>CA</t>
   </si>
   <si>
     <t>EDH</t>
@@ -47,16 +41,7 @@
     <t>IL</t>
   </si>
   <si>
-    <t>KHL</t>
-  </si>
-  <si>
-    <t>MA</t>
-  </si>
-  <si>
     <t>MLN</t>
-  </si>
-  <si>
-    <t>MN</t>
   </si>
   <si>
     <t>NC</t>
@@ -78,15 +63,6 @@
   </si>
   <si>
     <t>WI</t>
-  </si>
-  <si>
-    <t>ELN</t>
-  </si>
-  <si>
-    <t>FIF</t>
-  </si>
-  <si>
-    <t>NW</t>
   </si>
   <si>
     <t>State</t>
@@ -170,6 +146,37 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>#reviews</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -233,64 +240,40 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$20</c:f>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>AZ</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>BW</c:v>
+                  <c:v>EDH</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CA</c:v>
+                  <c:v>IL</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>EDH</c:v>
+                  <c:v>MLN</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>ELN</c:v>
+                  <c:v>NC</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>FIF</c:v>
+                  <c:v>NV</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>IL</c:v>
+                  <c:v>ON</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>KHL</c:v>
+                  <c:v>PA</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>MA</c:v>
+                  <c:v>QC</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>MLN</c:v>
+                  <c:v>SC</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>MN</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>NC</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>NV</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>NW</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>ON</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>PA</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>QC</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>SC</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>WI</c:v>
                 </c:pt>
               </c:strCache>
@@ -298,65 +281,41 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$20</c:f>
+              <c:f>Sheet1!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>7976.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.0</c:v>
+                  <c:v>366.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>182.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>366.0</c:v>
+                  <c:v>47.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>1356.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>10032.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>182.0</c:v>
+                  <c:v>93.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0</c:v>
+                  <c:v>1190.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0</c:v>
+                  <c:v>869.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>47.0</c:v>
+                  <c:v>63.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1356.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>10032.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>93.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1190.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>869.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>63.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>581.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -389,64 +348,40 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$20</c:f>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>AZ</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>BW</c:v>
+                  <c:v>EDH</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CA</c:v>
+                  <c:v>IL</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>EDH</c:v>
+                  <c:v>MLN</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>ELN</c:v>
+                  <c:v>NC</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>FIF</c:v>
+                  <c:v>NV</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>IL</c:v>
+                  <c:v>ON</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>KHL</c:v>
+                  <c:v>PA</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>MA</c:v>
+                  <c:v>QC</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>MLN</c:v>
+                  <c:v>SC</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>MN</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>NC</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>NV</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>NW</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>ON</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>PA</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>QC</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>SC</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>WI</c:v>
                 </c:pt>
               </c:strCache>
@@ -454,65 +389,41 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$20</c:f>
+              <c:f>Sheet1!$C$2:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>153430.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1162.0</c:v>
+                  <c:v>3774.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34.0</c:v>
+                  <c:v>2295.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3774.0</c:v>
+                  <c:v>603.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0</c:v>
+                  <c:v>26091.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.0</c:v>
+                  <c:v>168965.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2295.0</c:v>
+                  <c:v>1187.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.0</c:v>
+                  <c:v>18178.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.0</c:v>
+                  <c:v>15061.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>603.0</c:v>
+                  <c:v>1036.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>26091.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>168965.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1187.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>18178.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>15061.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1036.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>8161.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -529,11 +440,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2103022736"/>
-        <c:axId val="-2097510064"/>
+        <c:axId val="-2108476976"/>
+        <c:axId val="-2092391120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2103022736"/>
+        <c:axId val="-2108476976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -576,7 +487,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2097510064"/>
+        <c:crossAx val="-2092391120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -584,7 +495,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2097510064"/>
+        <c:axId val="-2092391120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -634,7 +545,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2103022736"/>
+        <c:crossAx val="-2108476976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -794,64 +705,40 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$20</c:f>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>AZ</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>BW</c:v>
+                  <c:v>EDH</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CA</c:v>
+                  <c:v>IL</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>EDH</c:v>
+                  <c:v>MLN</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>ELN</c:v>
+                  <c:v>NC</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>FIF</c:v>
+                  <c:v>NV</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>IL</c:v>
+                  <c:v>ON</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>KHL</c:v>
+                  <c:v>PA</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>MA</c:v>
+                  <c:v>QC</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>MLN</c:v>
+                  <c:v>SC</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>MN</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>NC</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>NV</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>NW</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>ON</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>PA</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>QC</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>SC</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>WI</c:v>
                 </c:pt>
               </c:strCache>
@@ -859,65 +746,41 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$20</c:f>
+              <c:f>Sheet1!$D$2:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.0519846183927524</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.00516351118760757</c:v>
+                  <c:v>0.0969793322734499</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.088235294117647</c:v>
+                  <c:v>0.0793028322440087</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0969793322734499</c:v>
+                  <c:v>0.0779436152570481</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0.051971944348626</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>0.0593732429793152</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0793028322440087</c:v>
+                  <c:v>0.0783487784330244</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.166666666666667</c:v>
+                  <c:v>0.0654637473869513</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.333333333333333</c:v>
+                  <c:v>0.0576986919859239</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0779436152570481</c:v>
+                  <c:v>0.0608108108108108</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.75</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.051971944348626</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.0593732429793152</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.0783487784330244</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.0654637473869513</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.0576986919859239</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.0608108108108108</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>0.0711922558509986</c:v>
                 </c:pt>
               </c:numCache>
@@ -934,11 +797,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2110727664"/>
-        <c:axId val="-2115985728"/>
+        <c:axId val="-2108154592"/>
+        <c:axId val="-2092174080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2110727664"/>
+        <c:axId val="-2108154592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -981,7 +844,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2115985728"/>
+        <c:crossAx val="-2092174080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -989,7 +852,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2115985728"/>
+        <c:axId val="-2092174080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1009,6 +872,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1039,7 +903,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2110727664"/>
+        <c:crossAx val="-2108154592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2194,15 +2058,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
+      <xdr:colOff>12699</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>43252</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2223,16 +2087,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>26</xdr:col>
+      <xdr:col>30</xdr:col>
       <xdr:colOff>12699</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>42</xdr:col>
-      <xdr:colOff>281516</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>61</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2517,10 +2381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2530,16 +2394,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2553,7 +2417,7 @@
         <v>153430</v>
       </c>
       <c r="D2" s="2">
-        <f>B2/C2</f>
+        <f t="shared" ref="D2:D12" si="0">B2/C2</f>
         <v>5.1984618392752396E-2</v>
       </c>
     </row>
@@ -2562,14 +2426,14 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>366</v>
       </c>
       <c r="C3">
-        <v>1162</v>
+        <v>3774</v>
       </c>
       <c r="D3" s="2">
-        <f>B3/C3</f>
-        <v>5.1635111876075735E-3</v>
+        <f t="shared" si="0"/>
+        <v>9.6979332273449917E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2577,14 +2441,14 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>182</v>
       </c>
       <c r="C4">
-        <v>34</v>
+        <v>2295</v>
       </c>
       <c r="D4" s="2">
-        <f>B4/C4</f>
-        <v>8.8235294117647065E-2</v>
+        <f t="shared" si="0"/>
+        <v>7.930283224400872E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -2592,238 +2456,118 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>366</v>
+        <v>47</v>
       </c>
       <c r="C5">
-        <v>3774</v>
+        <v>603</v>
       </c>
       <c r="D5" s="2">
-        <f>B5/C5</f>
-        <v>9.6979332273449917E-2</v>
+        <f t="shared" si="0"/>
+        <v>7.7943615257048099E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1356</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>26091</v>
       </c>
       <c r="D6" s="2">
-        <f>B6/C6</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>5.1971944348625961E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>10032</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>168965</v>
       </c>
       <c r="D7" s="2">
-        <f>B7/C7</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>5.937324297931524E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>182</v>
+        <v>93</v>
       </c>
       <c r="C8">
-        <v>2295</v>
+        <v>1187</v>
       </c>
       <c r="D8" s="2">
-        <f>B8/C8</f>
-        <v>7.930283224400872E-2</v>
+        <f t="shared" si="0"/>
+        <v>7.834877843302443E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>1190</v>
       </c>
       <c r="C9">
-        <v>6</v>
+        <v>18178</v>
       </c>
       <c r="D9" s="2">
-        <f>B9/C9</f>
-        <v>0.16666666666666666</v>
+        <f t="shared" si="0"/>
+        <v>6.5463747386951265E-2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>869</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>15061</v>
       </c>
       <c r="D10" s="2">
-        <f>B10/C10</f>
-        <v>0.33333333333333331</v>
+        <f t="shared" si="0"/>
+        <v>5.7698691985923908E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="C11">
-        <v>603</v>
+        <v>1036</v>
       </c>
       <c r="D11" s="2">
-        <f>B11/C11</f>
-        <v>7.7943615257048099E-2</v>
+        <f t="shared" si="0"/>
+        <v>6.0810810810810814E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>581</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>8161</v>
       </c>
       <c r="D12" s="2">
-        <f>B12/C12</f>
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13">
-        <v>1356</v>
-      </c>
-      <c r="C13">
-        <v>26091</v>
-      </c>
-      <c r="D13" s="2">
-        <f>B13/C13</f>
-        <v>5.1971944348625961E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14">
-        <v>10032</v>
-      </c>
-      <c r="C14">
-        <v>168965</v>
-      </c>
-      <c r="D14" s="2">
-        <f>B14/C14</f>
-        <v>5.937324297931524E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="D15" s="2">
-        <f>B15/C15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16">
-        <v>93</v>
-      </c>
-      <c r="C16">
-        <v>1187</v>
-      </c>
-      <c r="D16" s="2">
-        <f>B16/C16</f>
-        <v>7.834877843302443E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17">
-        <v>1190</v>
-      </c>
-      <c r="C17">
-        <v>18178</v>
-      </c>
-      <c r="D17" s="2">
-        <f>B17/C17</f>
-        <v>6.5463747386951265E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18">
-        <v>869</v>
-      </c>
-      <c r="C18">
-        <v>15061</v>
-      </c>
-      <c r="D18" s="2">
-        <f>B18/C18</f>
-        <v>5.7698691985923908E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19">
-        <v>63</v>
-      </c>
-      <c r="C19">
-        <v>1036</v>
-      </c>
-      <c r="D19" s="2">
-        <f>B19/C19</f>
-        <v>6.0810810810810814E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20">
-        <v>581</v>
-      </c>
-      <c r="C20">
-        <v>8161</v>
-      </c>
-      <c r="D20" s="2">
-        <f>B20/C20</f>
+        <f t="shared" si="0"/>
         <v>7.1192255850998656E-2</v>
       </c>
     </row>

</xml_diff>